<commit_message>
Most recent CPU, trying to fix load instruction
</commit_message>
<xml_diff>
--- a/ROM Spreadsheet.xlsx
+++ b/ROM Spreadsheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10120" yWindow="920" windowWidth="26960" windowHeight="17380" tabRatio="500"/>
+    <workbookView xWindow="9420" yWindow="2960" windowWidth="26960" windowHeight="17380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
   <si>
     <t>Hex Address</t>
   </si>
@@ -180,6 +180,45 @@
   </si>
   <si>
     <t>Halt execution</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>JUMP</t>
+  </si>
+  <si>
+    <t>LOAD A</t>
+  </si>
+  <si>
+    <t>MOV B,A</t>
+  </si>
+  <si>
+    <t>ADD A,B</t>
+  </si>
+  <si>
+    <t>A AND B</t>
+  </si>
+  <si>
+    <t>A AND B, Store in Reg A</t>
+  </si>
+  <si>
+    <t>A AND B HELPER</t>
+  </si>
+  <si>
+    <t>A OR B</t>
+  </si>
+  <si>
+    <t>A OR B, Store in Reg B</t>
+  </si>
+  <si>
+    <t>A OR B HELPER</t>
+  </si>
+  <si>
+    <t>0A</t>
+  </si>
+  <si>
+    <t>0B</t>
   </si>
 </sst>
 </file>
@@ -195,15 +234,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -211,12 +262,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,7 +596,7 @@
     <col min="17" max="17" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -564,7 +652,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -623,7 +711,7 @@
         <v>04</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -682,8 +770,14 @@
         <f t="shared" ref="R3:R33" si="1">BIN2HEX(CONCATENATE(H3,I3,J3,K3,L3,M3,N3,O3),2)</f>
         <v>00</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -742,8 +836,15 @@
         <f t="shared" si="1"/>
         <v>E0</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T4" s="4" t="str">
+        <f>HEX2BIN(1, 2)</f>
+        <v>01</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -802,8 +903,15 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T5" s="3" t="str">
+        <f>DEC2HEX(T4+1,2)</f>
+        <v>02</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -862,8 +970,15 @@
         <f t="shared" si="1"/>
         <v>A4</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T6" s="3" t="str">
+        <f t="shared" ref="T6:T12" si="4">DEC2HEX(T5+1,2)</f>
+        <v>03</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -922,8 +1037,15 @@
         <f t="shared" si="1"/>
         <v>A4</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T7" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>04</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -982,8 +1104,15 @@
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T8" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>05</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1042,8 +1171,15 @@
         <f t="shared" si="1"/>
         <v>02</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T9" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>06</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1102,8 +1238,15 @@
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T10" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v>07</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1162,8 +1305,18 @@
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T11" s="3" t="str">
+        <f>DEC2HEX(T10+1,2)</f>
+        <v>08</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
       <c r="B12" t="str">
         <f t="shared" si="2"/>
         <v>0A</v>
@@ -1172,16 +1325,65 @@
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
+      <c r="D12">
+        <v>21</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>57</v>
+      </c>
       <c r="Q12" t="str">
         <f t="shared" si="0"/>
-        <v>00</v>
+        <v>AB</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T12" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>09</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
       <c r="B13" t="str">
         <f t="shared" si="2"/>
         <v>0B</v>
@@ -1190,16 +1392,61 @@
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
+      <c r="D13">
+        <v>22</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13" t="s">
+        <v>60</v>
+      </c>
       <c r="Q13" t="str">
         <f t="shared" si="0"/>
-        <v>00</v>
+        <v>B3</v>
       </c>
       <c r="R13" t="str">
         <f t="shared" si="1"/>
-        <v>00</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B14" t="str">
         <f t="shared" si="2"/>
         <v>0C</v>
@@ -1216,8 +1463,14 @@
         <f t="shared" si="1"/>
         <v>00</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="T14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B15" t="str">
         <f t="shared" si="2"/>
         <v>0D</v>
@@ -1235,7 +1488,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B16" t="str">
         <f t="shared" si="2"/>
         <v>0E</v>
@@ -1431,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20">
         <v>0</v>
@@ -1448,7 +1701,7 @@
       </c>
       <c r="R20" t="str">
         <f t="shared" si="1"/>
-        <v>A1</v>
+        <v>A5</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
@@ -1572,6 +1825,9 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
       <c r="B23" t="str">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -1580,16 +1836,58 @@
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23" t="s">
+        <v>29</v>
+      </c>
       <c r="Q23" t="str">
         <f t="shared" si="0"/>
-        <v>00</v>
+        <v>03</v>
       </c>
       <c r="R23" t="str">
         <f t="shared" si="1"/>
-        <v>00</v>
+        <v>01</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
       <c r="B24" t="str">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -1598,13 +1896,52 @@
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24" t="s">
+        <v>29</v>
+      </c>
       <c r="Q24" t="str">
         <f t="shared" si="0"/>
-        <v>00</v>
+        <v>03</v>
       </c>
       <c r="R24" t="str">
         <f t="shared" si="1"/>
-        <v>00</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>